<commit_message>
remove link from 吴顺祥
</commit_message>
<xml_diff>
--- a/previous/data20210326.xlsx
+++ b/previous/data20210326.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dehaiwu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuyue\Documents\GitHub\WuGenealogy\previous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F7ACA8-96C4-234B-BC9A-28C1EA9AD94B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B91C8-F266-4E01-BB46-43679B04BB87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="500" windowWidth="17380" windowHeight="15860" xr2:uid="{BE040026-2525-2F41-8154-13C10946EE35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE040026-2525-2F41-8154-13C10946EE35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -70,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>吴顺祥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>八世</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1094,7 +1090,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1150,7 +1146,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1191,7 +1187,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1217,7 +1213,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1643,7 +1639,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2309,7 +2305,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2354,7 +2350,7 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -2446,6 +2442,9 @@
     <t>吴兆胜
 李惠玲</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吴顺祥&lt;nolink&gt;</t>
   </si>
 </sst>
 </file>
@@ -2456,14 +2455,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2471,7 +2470,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2485,7 +2484,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2493,7 +2492,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2501,7 +2500,7 @@
     <font>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2587,7 +2586,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2603,7 +2602,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2901,20 +2900,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C2917E-BE49-8D43-B460-AF3709AE4A60}">
   <dimension ref="A1:L225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C208" zoomScale="158" workbookViewId="0">
-      <selection activeCell="F214" sqref="F214"/>
+    <sheetView tabSelected="1" topLeftCell="C214" zoomScale="158" workbookViewId="0">
+      <selection activeCell="I230" sqref="I230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2940,27 +2939,27 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="28">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="25.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -2969,26 +2968,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28">
+    <row r="3" spans="1:12" ht="25.5">
       <c r="C3" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>278</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28">
+    <row r="4" spans="1:12" ht="25.5">
       <c r="E4" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
@@ -3002,1897 +3001,1897 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="28">
+    <row r="6" spans="1:12" ht="25.5">
       <c r="F6" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28">
+    <row r="7" spans="1:12" ht="25.5">
       <c r="H7" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="J8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="K9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="J10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="J11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="25.5">
       <c r="I12" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>370</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="K13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="K14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="J15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="J16" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" ht="25.5">
+      <c r="I17" s="5" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="17" spans="7:11" ht="28">
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>373</v>
-      </c>
       <c r="K17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="7:11">
       <c r="J18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="7:11" ht="28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" ht="25.5">
       <c r="I19" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="7:11">
       <c r="J20" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="7:11" ht="28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" ht="25.5">
       <c r="G21" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="7:11" ht="28">
+    <row r="22" spans="7:11" ht="25.5">
       <c r="H22" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="7:11">
       <c r="K23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="7:11">
       <c r="J24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="7:11" ht="28">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="7:11" ht="25.5">
       <c r="H25" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="7:11" ht="28">
+    <row r="26" spans="7:11" ht="25.5">
       <c r="G26" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="7:11">
       <c r="K27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="7:11">
       <c r="J28" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="7:11">
       <c r="K29" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="7:11">
       <c r="J30" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="7:11">
       <c r="K31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="7:11">
       <c r="J32" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="6:12">
       <c r="J33" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="34" spans="6:12" ht="28">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="6:12" ht="25.5">
       <c r="I34" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="35" spans="6:12">
       <c r="J35" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12" ht="25.5">
+      <c r="H36" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="36" spans="6:12" ht="28">
-      <c r="H36" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="K36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="6:12">
       <c r="J37" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="6:12" ht="40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="6:12" ht="34.5">
       <c r="H38" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I38" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="K38" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="6:12">
       <c r="J39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="6:12">
       <c r="J40" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="6:12" ht="28">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12" ht="25.5">
       <c r="H41" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="6:12">
       <c r="K42" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12" ht="25.5">
+      <c r="I43" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="6:12" ht="28">
-      <c r="I43" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="44" spans="6:12">
       <c r="J44" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="6:12" ht="32.25">
+      <c r="F45" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="45" spans="6:12" ht="37">
-      <c r="F45" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="G45" s="5" t="s">
+      <c r="K45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="6:12">
+      <c r="J46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="6:12" ht="25.5">
+      <c r="G47" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="H45" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="I45" s="5" t="s">
+      <c r="H47" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="I47" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K45" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="6:12" ht="14">
-      <c r="J46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="47" spans="6:12" ht="28">
-      <c r="G47" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>327</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="K47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="6:12">
       <c r="J48" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="7:12">
       <c r="J49" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="7:12">
       <c r="J50" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="7:12" ht="28">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="7:12" ht="25.5">
       <c r="I51" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="7:12">
       <c r="J52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="7:12">
       <c r="J53" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="7:12" ht="25.5">
+      <c r="H54" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="7:12" ht="28">
-      <c r="H54" s="5" t="s">
+    <row r="55" spans="7:12" ht="25.5">
+      <c r="I55" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="7:12" ht="28">
-      <c r="I55" s="5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="56" spans="7:12" ht="37">
+    </row>
+    <row r="56" spans="7:12" ht="32.25">
       <c r="H56" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J56" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K56" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="57" spans="7:12">
       <c r="J57" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="58" spans="7:12" ht="28">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="58" spans="7:12" ht="25.5">
       <c r="I58" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="J58" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="59" spans="7:12">
       <c r="J59" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="7:12" ht="34.5">
+      <c r="I60" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="7:12" ht="39">
-      <c r="I60" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="J60" s="1" t="s">
+    <row r="61" spans="7:12" ht="25.5">
+      <c r="H61" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="61" spans="7:12" ht="28">
-      <c r="H61" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="62" spans="7:12">
       <c r="I62" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="7:12" ht="25.5">
+      <c r="G63" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="63" spans="7:12" ht="28">
-      <c r="G63" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="7:12">
       <c r="J64" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L64" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="L64" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="65" spans="5:12">
       <c r="J65" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="5:12" ht="28">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="5:12" ht="25.5">
       <c r="H66" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="5:12" ht="25.5">
+      <c r="I67" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="5:12" ht="38.25">
+      <c r="E68" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H68" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="I66" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="67" spans="5:12" ht="28">
-      <c r="I67" s="5" t="s">
+    </row>
+    <row r="69" spans="5:12" ht="25.5">
+      <c r="H69" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="I69" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="J69" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="68" spans="5:12" ht="42">
-      <c r="E68" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="H68" s="5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="69" spans="5:12" ht="29">
-      <c r="H69" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="I69" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="K69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="5:12">
       <c r="J70" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L70" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="71" spans="5:12">
       <c r="J71" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="5:12">
       <c r="K72" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="5:12">
       <c r="J73" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L73" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="74" spans="5:12" ht="25.5">
+      <c r="I74" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="K74" s="1" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="74" spans="5:12" ht="28">
-      <c r="I74" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="75" spans="5:12">
       <c r="K75" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="5:12" ht="25.5">
+      <c r="G76" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="J76" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="76" spans="5:12" ht="28">
-      <c r="G76" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="I76" s="5" t="s">
+      <c r="K76" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="5:12">
+      <c r="K77" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="78" spans="5:12" ht="25.5">
+      <c r="I78" s="5" t="s">
         <v>403</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K76" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="5:12" ht="14">
-      <c r="K77" s="1" t="s">
+    </row>
+    <row r="79" spans="5:12" ht="25.5">
+      <c r="I79" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="J79" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L77" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="78" spans="5:12" ht="28">
-      <c r="I78" s="5" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="79" spans="5:12" ht="28">
-      <c r="I79" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="K79" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="5:12">
       <c r="J80" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K80" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L80" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="81" spans="7:12">
       <c r="K81" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="7:12" ht="25.5">
+      <c r="H82" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="83" spans="7:12" ht="25.5">
+      <c r="G83" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="J83" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="82" spans="7:12" ht="28">
-      <c r="H82" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="83" spans="7:12" ht="28">
-      <c r="G83" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="I83" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="K83" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L83" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="84" spans="7:12">
       <c r="J84" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="85" spans="7:12">
       <c r="K85" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="7:12">
       <c r="J86" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K86" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="K86" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="87" spans="7:12" ht="14">
+    </row>
+    <row r="87" spans="7:12">
       <c r="K87" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88" spans="7:12">
       <c r="J88" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="7:12">
       <c r="J89" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K89" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L89" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="L89" s="1" t="s">
+    </row>
+    <row r="90" spans="7:12" ht="25.5">
+      <c r="I90" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="J90" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="90" spans="7:12" ht="28">
-      <c r="I90" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="J90" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="K90" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="7:12">
       <c r="J91" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="7:12">
       <c r="J92" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="7:12">
       <c r="K93" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="94" spans="7:12" ht="28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="7:12" ht="25.5">
       <c r="H94" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I94" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="7:12" ht="25.5">
+      <c r="I95" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="J94" s="1" t="s">
+      <c r="J95" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="95" spans="7:12" ht="28">
-      <c r="I95" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="J95" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="K95" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="96" spans="7:12">
       <c r="J96" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="7:11">
       <c r="J97" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="98" spans="7:11" ht="28">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="98" spans="7:11" ht="25.5">
       <c r="I98" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="7:11">
       <c r="J99" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="7:11">
       <c r="J100" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="7:11" ht="25.5">
+      <c r="H101" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="J101" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="101" spans="7:11" ht="28">
-      <c r="H101" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="I101" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="J101" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="102" spans="7:11">
       <c r="J102" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="103" spans="7:11" ht="25.5">
+      <c r="H103" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="I103" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="J103" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="104" spans="7:11" ht="25.5">
+      <c r="I104" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="J104" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="103" spans="7:11" ht="28">
-      <c r="H103" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="I103" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="J103" s="5" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="104" spans="7:11" ht="28">
-      <c r="I104" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="K104" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="7:11">
       <c r="I105" s="5"/>
       <c r="J105" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="106" spans="7:11" ht="25.5">
+      <c r="I106" s="5" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="106" spans="7:11" ht="28">
-      <c r="I106" s="5" t="s">
+      <c r="J106" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="7:11" ht="25.5">
+      <c r="I107" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="J106" s="1" t="s">
+      <c r="J107" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="107" spans="7:11" ht="28">
-      <c r="I107" s="5" t="s">
+      <c r="K107" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="108" spans="7:11" ht="25.5">
+      <c r="I108" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="J107" s="1" t="s">
+      <c r="J108" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K107" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="108" spans="7:11" ht="28">
-      <c r="I108" s="5" t="s">
+      <c r="K108" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="109" spans="7:11" ht="32.25">
+      <c r="G109" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="H109" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="I109" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="J108" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="K108" s="1" t="s">
+      <c r="J109" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K109" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="7:11" ht="37">
-      <c r="G109" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="H109" s="5" t="s">
+    <row r="110" spans="7:11" ht="25.5">
+      <c r="H110" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="I109" s="5" t="s">
+      <c r="I110" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="J109" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="K109" s="1" t="s">
+      <c r="J110" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="110" spans="7:11" ht="28">
-      <c r="H110" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="I110" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="J110" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="K110" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="7:11">
       <c r="K111" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="7:11">
       <c r="J112" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="6:11">
       <c r="J113" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="114" spans="6:11" ht="28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="6:11" ht="25.5">
       <c r="G114" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H114" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="115" spans="6:11" ht="25.5">
+      <c r="I115" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="6:11" ht="25.5">
+      <c r="H116" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="I114" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="115" spans="6:11" ht="29">
-      <c r="I115" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="116" spans="6:11" ht="28">
-      <c r="H116" s="5" t="s">
-        <v>347</v>
-      </c>
       <c r="I116" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="6:11">
       <c r="J117" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K117" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="K117" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="118" spans="6:11">
       <c r="K118" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="119" spans="6:11" ht="28">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="119" spans="6:11" ht="25.5">
       <c r="I119" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="120" spans="6:11">
       <c r="J120" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="121" spans="6:11" ht="28">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="121" spans="6:11" ht="25.5">
       <c r="F121" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H121" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="122" spans="6:11">
       <c r="J122" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="123" spans="6:11">
       <c r="J123" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K123" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="124" spans="6:11" ht="25.5">
+      <c r="I124" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="J124" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="124" spans="6:11" ht="28">
-      <c r="I124" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="J124" s="1" t="s">
+      <c r="K124" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="K124" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="125" spans="6:11">
       <c r="J125" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K125" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126" spans="6:11" ht="25.5">
+      <c r="I126" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="J126" s="1" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="126" spans="6:11" ht="28">
-      <c r="I126" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="127" spans="6:11">
       <c r="J127" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="6:11">
       <c r="J128" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="4:12">
       <c r="I129" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="4:12">
       <c r="H130" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131" spans="4:12">
       <c r="H131" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="132" spans="4:12">
       <c r="H132" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="133" spans="4:12" ht="28">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="133" spans="4:12" ht="25.5">
       <c r="G133" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="134" spans="4:12">
       <c r="H134" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I134" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="I134" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="135" spans="4:12" ht="42">
+    </row>
+    <row r="135" spans="4:12" ht="35.25">
       <c r="D135" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I135" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="136" spans="4:12" ht="25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="136" spans="4:12" ht="21.75">
       <c r="J136" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="137" spans="4:12">
       <c r="J137" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="138" spans="4:12">
       <c r="J138" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="139" spans="4:12" ht="28">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="139" spans="4:12" ht="25.5">
       <c r="I139" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J139" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K139" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K139" s="1" t="s">
+      <c r="L139" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="L139" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="140" spans="4:12">
       <c r="K140" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="141" spans="4:12">
       <c r="J141" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="142" spans="4:12">
       <c r="K142" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="143" spans="4:12">
       <c r="J143" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K143" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="K143" s="1" t="s">
+      <c r="L143" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="L143" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="144" spans="4:12">
       <c r="J144" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K144" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="K144" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="145" spans="6:12">
       <c r="K145" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="6:12">
       <c r="J146" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="147" spans="6:12">
       <c r="J147" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="6:12">
       <c r="J148" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="149" spans="6:12" ht="25.5">
+      <c r="I149" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="J149" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="149" spans="6:12" ht="28">
-      <c r="I149" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="J149" s="1" t="s">
+      <c r="K149" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L149" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="K149" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L149" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="150" spans="6:12">
       <c r="L150" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="151" spans="6:12">
       <c r="J151" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="152" spans="6:12">
       <c r="J152" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="153" spans="6:12">
       <c r="I153" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="154" spans="6:12">
       <c r="I154" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="155" spans="6:12" ht="25.5">
+      <c r="H155" s="5" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="155" spans="6:12" ht="28">
-      <c r="H155" s="5" t="s">
+      <c r="I155" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="156" spans="6:12" ht="25.5">
+      <c r="H156" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="I155" s="1" t="s">
+      <c r="I156" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="157" spans="6:12" ht="25.5">
+      <c r="F157" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H157" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="158" spans="6:12" ht="33.75">
+      <c r="F158" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="H158" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="I158" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="J158" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="156" spans="6:12" ht="28">
-      <c r="H156" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="I156" s="5" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="157" spans="6:12" ht="28">
-      <c r="F157" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="G157" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="H157" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="158" spans="6:12" ht="40">
-      <c r="F158" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="G158" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="H158" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="I158" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="J158" s="1" t="s">
+      <c r="K158" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="K158" s="1" t="s">
+      <c r="L158" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="L158" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="159" spans="6:12">
       <c r="J159" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="160" spans="6:12" ht="25.5">
+      <c r="I160" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="J160" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="160" spans="6:12" ht="28">
-      <c r="I160" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="J160" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="K160" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L160" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="L160" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="161" spans="5:12">
       <c r="J161" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="162" spans="5:12">
       <c r="J162" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="163" spans="5:12" ht="40">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="163" spans="5:12" ht="33.75">
       <c r="I163" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="164" spans="5:12">
       <c r="J164" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="165" spans="5:12" ht="25.5">
+      <c r="I165" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="J165" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="165" spans="5:12" ht="28">
-      <c r="I165" s="5" t="s">
+      <c r="K165" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="166" spans="5:12" ht="25.5">
+      <c r="I166" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="J165" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="K165" s="1" t="s">
+      <c r="J166" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="166" spans="5:12" ht="28">
-      <c r="I166" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="J166" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="K166" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="167" spans="5:12">
+      <c r="K167" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="167" spans="5:12" ht="14">
-      <c r="K167" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="168" spans="5:12" ht="28">
+    <row r="168" spans="5:12" ht="25.5">
       <c r="E168" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F168" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G168" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="5:12" ht="28">
+    <row r="169" spans="5:12" ht="25.5">
       <c r="E169" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F169" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G169" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I169" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="170" spans="5:12">
       <c r="J170" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K170" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="K170" s="1" t="s">
+      <c r="L170" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="L170" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="171" spans="5:12">
       <c r="L171" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="172" spans="5:12">
       <c r="J172" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="173" spans="5:12" ht="25.5">
+      <c r="I173" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="J173" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="K172" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="173" spans="5:12" ht="28">
-      <c r="I173" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="J173" s="1" t="s">
+      <c r="K173" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="K173" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="174" spans="5:12">
       <c r="J174" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="175" spans="5:12" ht="25.5">
+      <c r="I175" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K175" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="175" spans="5:12" ht="28">
-      <c r="I175" s="5" t="s">
+    <row r="176" spans="5:12" ht="25.5">
+      <c r="H176" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="I176" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="J175" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K175" s="1" t="s">
+      <c r="J176" s="1" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="176" spans="5:12" ht="28">
-      <c r="H176" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="I176" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="J176" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="177" spans="7:11">
       <c r="J177" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="178" spans="7:11" ht="25.5">
+      <c r="I178" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="J178" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="178" spans="7:11" ht="29">
-      <c r="I178" s="5" t="s">
+      <c r="K178" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="179" spans="7:11" ht="25.5">
+      <c r="H179" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="I179" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="J178" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="K178" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="179" spans="7:11" ht="28">
-      <c r="H179" s="5" t="s">
+      <c r="J179" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="180" spans="7:11" ht="25.5">
+      <c r="I180" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="J180" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="181" spans="7:11">
+      <c r="I181" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="I179" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="J179" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="180" spans="7:11" ht="28">
-      <c r="I180" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="J180" s="1" t="s">
+    </row>
+    <row r="182" spans="7:11">
+      <c r="I182" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="183" spans="7:11" ht="25.5">
+      <c r="H183" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="I183" s="5" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="181" spans="7:11" ht="14">
-      <c r="I181" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="182" spans="7:11" ht="14">
-      <c r="I182" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="183" spans="7:11" ht="29">
-      <c r="H183" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="I183" s="5" t="s">
-        <v>448</v>
-      </c>
       <c r="J183" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="184" spans="7:11">
       <c r="J184" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="185" spans="7:11">
       <c r="I185" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="186" spans="7:11" ht="28">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="186" spans="7:11" ht="25.5">
       <c r="G186" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="187" spans="7:11">
       <c r="H187" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="188" spans="7:11" ht="25.5">
+      <c r="G188" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="H188" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="I188" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="J188" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="188" spans="7:11" ht="28">
-      <c r="G188" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="H188" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="I188" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="J188" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="K188" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="189" spans="7:11">
       <c r="J189" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="K189" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="K189" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="190" spans="7:11" ht="14">
+    </row>
+    <row r="190" spans="7:11">
       <c r="K190" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="191" spans="7:11">
       <c r="J191" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="192" spans="7:11" ht="25.5">
+      <c r="I192" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="J192" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="192" spans="7:11" ht="28">
-      <c r="I192" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="J192" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="K192" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="193" spans="8:11">
       <c r="K193" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="194" spans="8:11">
       <c r="J194" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K194" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="195" spans="8:11">
       <c r="I195" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="196" spans="8:11" ht="25.5">
+      <c r="I196" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="J196" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="196" spans="8:11" ht="28">
-      <c r="I196" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="J196" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="K196" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="197" spans="8:11">
       <c r="J197" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K197" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="198" spans="8:11" ht="25.5">
+      <c r="I198" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="J198" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="198" spans="8:11" ht="28">
-      <c r="I198" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="J198" s="1" t="s">
+      <c r="K198" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="K198" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="199" spans="8:11">
       <c r="J199" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K199" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="200" spans="8:11" ht="25.5">
+      <c r="I200" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="J200" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="200" spans="8:11" ht="28">
-      <c r="I200" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="J200" s="1" t="s">
+      <c r="K200" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="K200" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="201" spans="8:11">
       <c r="J201" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="202" spans="8:11">
       <c r="I202" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="203" spans="8:11" ht="28">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="203" spans="8:11" ht="25.5">
       <c r="H203" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I203" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J203" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K203" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="204" spans="8:11">
       <c r="J204" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="K204" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="K204" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="205" spans="8:11">
       <c r="J205" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="206" spans="8:11">
       <c r="I206" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="207" spans="8:11">
       <c r="I207" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="208" spans="8:11" ht="25.5">
+      <c r="H208" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="I208" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="J208" s="1" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="208" spans="8:11" ht="28">
-      <c r="H208" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="I208" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="J208" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="209" spans="7:11">
       <c r="J209" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="210" spans="7:11" ht="25.5">
+      <c r="G210" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H210" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="I210" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="J210" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="210" spans="7:11" ht="28">
-      <c r="G210" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="H210" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="I210" s="5" t="s">
+      <c r="K210" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="211" spans="7:11" ht="25.5">
+      <c r="I211" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="J210" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="K210" s="1" t="s">
+      <c r="J211" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="211" spans="7:11" ht="28">
-      <c r="I211" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="J211" s="1" t="s">
+      <c r="K211" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="K211" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="212" spans="7:11">
       <c r="K212" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="213" spans="7:11" ht="25.5">
+      <c r="I213" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="J213" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="213" spans="7:11" ht="28">
-      <c r="I213" s="5" t="s">
+      <c r="K213" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="214" spans="7:11" ht="25.5">
+      <c r="I214" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="J213" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="K213" s="1" t="s">
+      <c r="J214" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="214" spans="7:11" ht="28">
-      <c r="I214" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="J214" s="1" t="s">
-        <v>249</v>
-      </c>
       <c r="K214" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="215" spans="7:11">
       <c r="J215" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="216" spans="7:11" ht="25.5">
+      <c r="I216" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="J216" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="216" spans="7:11" ht="28">
-      <c r="I216" s="5" t="s">
+      <c r="K216" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="217" spans="7:11" ht="25.5">
+      <c r="I217" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="J216" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="K216" s="1" t="s">
+      <c r="J217" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="217" spans="7:11" ht="28">
-      <c r="I217" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="J217" s="1" t="s">
+      <c r="K217" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="K217" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="218" spans="7:11">
       <c r="J218" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="219" spans="7:11" ht="25.5">
+      <c r="G219" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="H219" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="I219" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="J219" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="219" spans="7:11" ht="28">
-      <c r="G219" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="H219" s="5" t="s">
+    <row r="220" spans="7:11" ht="25.5">
+      <c r="H220" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="I219" s="5" t="s">
+      <c r="I220" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="J219" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="220" spans="7:11" ht="28">
-      <c r="H220" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="I220" s="5" t="s">
+      <c r="J220" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="J220" s="1" t="s">
+      <c r="K220" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="221" spans="7:11" ht="25.5">
+      <c r="I221" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="K220" s="1" t="s">
+      <c r="J221" s="1" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="221" spans="7:11" ht="28">
-      <c r="I221" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="J221" s="1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="222" spans="7:11">
       <c r="I222" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="223" spans="7:11">
       <c r="G223" s="1" t="s">
-        <v>11</v>
+        <v>465</v>
       </c>
       <c r="H223" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I223" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="224" spans="7:11">
       <c r="I224" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="225" spans="8:8">
       <c r="H225" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>